<commit_message>
candy alu file structure
</commit_message>
<xml_diff>
--- a/doc/24B-ISA.xlsx
+++ b/doc/24B-ISA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\haozi\Nextcloud\Share\vv\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cathe\Documents\vlsi-cpu\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48CB1EAD-D539-4D76-A4E6-C0B13746FE89}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC8B378B-5EE5-4601-8955-1EDF49DCE559}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" activeTab="3" xr2:uid="{300FB89C-001C-4516-AA49-DF67C212701F}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12168" xr2:uid="{300FB89C-001C-4516-AA49-DF67C212701F}"/>
   </bookViews>
   <sheets>
     <sheet name="Inst" sheetId="1" r:id="rId1"/>
@@ -822,37 +822,58 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -861,16 +882,22 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -886,7 +913,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1184,22 +1211,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBF12222-62EB-419B-868A-3559C151B634}">
   <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="9" style="1"/>
-    <col min="2" max="2" width="31.625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="31.6640625" style="1" customWidth="1"/>
     <col min="3" max="3" width="9" style="1"/>
-    <col min="4" max="4" width="12.125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12.109375" style="1" customWidth="1"/>
     <col min="5" max="5" width="9" style="1"/>
-    <col min="6" max="6" width="24.125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="24.109375" style="1" customWidth="1"/>
     <col min="7" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1219,638 +1246,638 @@
         <v>196</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:6">
+      <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="3" t="s">
         <v>179</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:6">
+      <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="3" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:6">
+      <c r="A4" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="3" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:6">
+      <c r="A5" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="3" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
+    <row r="6" spans="1:6">
+      <c r="A6" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="3" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:6">
+      <c r="A7" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="3" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
+    <row r="8" spans="1:6">
+      <c r="A8" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" s="3" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
+    <row r="9" spans="1:6">
+      <c r="A9" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" s="3" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
+    <row r="10" spans="1:6">
+      <c r="A10" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E10" s="3" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
+    <row r="11" spans="1:6">
+      <c r="A11" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E11" s="3" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
+    <row r="12" spans="1:6">
+      <c r="A12" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E12" s="3" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
+    <row r="13" spans="1:6">
+      <c r="A13" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E13" s="3" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
+    <row r="14" spans="1:6">
+      <c r="A14" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D14" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="E14" s="3" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
+    <row r="15" spans="1:6">
+      <c r="A15" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D15" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="E15" s="3" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
+    <row r="16" spans="1:6">
+      <c r="A16" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D16" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="E16" s="3" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
+    <row r="17" spans="1:5">
+      <c r="A17" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D17" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="E17" s="3" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
+    <row r="18" spans="1:5">
+      <c r="A18" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D18" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="E18" s="3" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
+    <row r="19" spans="1:5">
+      <c r="A19" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C19" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D19" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="E19" s="3" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
+    <row r="20" spans="1:5">
+      <c r="A20" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C20" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="D20" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="E20" s="3" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
+    <row r="21" spans="1:5">
+      <c r="A21" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C21" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="D21" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="E21" s="3" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="1" t="s">
+    <row r="22" spans="1:5">
+      <c r="A22" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C22" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="D22" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="E22" s="2" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="s">
+    <row r="23" spans="1:5">
+      <c r="A23" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C23" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="D23" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="E23" s="2" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" s="1" t="s">
+    <row r="24" spans="1:5">
+      <c r="A24" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C24" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="D24" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="E24" s="2" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" s="1" t="s">
+    <row r="25" spans="1:5">
+      <c r="A25" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B25" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="C25" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="D25" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="E25" s="2" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="s">
+    <row r="26" spans="1:5">
+      <c r="A26" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B26" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C26" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="D26" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="E26" s="1" t="s">
+      <c r="E26" s="2" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" s="1" t="s">
+    <row r="27" spans="1:5">
+      <c r="A27" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B27" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="C27" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="D27" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="E27" s="1" t="s">
+      <c r="E27" s="2" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" s="1" t="s">
+    <row r="28" spans="1:5">
+      <c r="A28" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B28" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C28" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="D28" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="E28" s="1" t="s">
+      <c r="E28" s="2" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" s="1" t="s">
+    <row r="29" spans="1:5">
+      <c r="A29" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B29" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="C29" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="D29" s="1" t="s">
+      <c r="D29" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="E29" s="2" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A30" s="1" t="s">
+    <row r="30" spans="1:5">
+      <c r="A30" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B30" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="C30" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="D30" s="1" t="s">
+      <c r="D30" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="E30" s="1" t="s">
+      <c r="E30" s="2" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A31" s="1" t="s">
+    <row r="31" spans="1:5">
+      <c r="A31" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B31" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C31" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="D31" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="E31" s="1" t="s">
+      <c r="E31" s="2" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A32" s="1" t="s">
+    <row r="32" spans="1:5">
+      <c r="A32" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B32" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="C32" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="D32" s="1" t="s">
+      <c r="D32" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="E32" s="1" t="s">
+      <c r="E32" s="2" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A33" s="1" t="s">
+    <row r="33" spans="1:6">
+      <c r="A33" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B33" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="C33" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="D33" s="1" t="s">
+      <c r="D33" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="E33" s="1" t="s">
+      <c r="E33" s="2" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A34" s="1" t="s">
+    <row r="34" spans="1:6">
+      <c r="A34" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B34" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="C34" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="D34" s="1" t="s">
+      <c r="D34" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="E34" s="1" t="s">
+      <c r="E34" s="2" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A35" s="1" t="s">
+    <row r="35" spans="1:6">
+      <c r="A35" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B35" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="C35" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="D35" s="1" t="s">
+      <c r="D35" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="E35" s="1" t="s">
+      <c r="E35" s="2" t="s">
         <v>190</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A36" s="1" t="s">
+    <row r="36" spans="1:6">
+      <c r="A36" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="B36" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="C36" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="D36" s="1" t="s">
+      <c r="D36" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="E36" s="1" t="s">
+      <c r="E36" s="2" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A37" s="1" t="s">
+    <row r="37" spans="1:6">
+      <c r="A37" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="B37" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="C37" s="1" t="s">
+      <c r="C37" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="D37" s="1" t="s">
+      <c r="D37" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="E37" s="1" t="s">
+      <c r="E37" s="2" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A38" s="1" t="s">
+    <row r="38" spans="1:6">
+      <c r="A38" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="B38" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="C38" s="1" t="s">
+      <c r="C38" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="D38" s="1" t="s">
+      <c r="D38" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="E38" s="1" t="s">
+      <c r="E38" s="2" t="s">
         <v>176</v>
       </c>
     </row>
@@ -1870,12 +1897,12 @@
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="18.25" customWidth="1"/>
+    <col min="1" max="1" width="18.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>75</v>
       </c>
@@ -1896,7 +1923,7 @@
       </c>
       <c r="G1" s="1"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7">
       <c r="A2" s="1" t="s">
         <v>81</v>
       </c>
@@ -1917,7 +1944,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7">
       <c r="A3" s="1" t="s">
         <v>83</v>
       </c>
@@ -1938,7 +1965,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7">
       <c r="A4" s="1" t="s">
         <v>84</v>
       </c>
@@ -1959,7 +1986,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7">
       <c r="A5" s="1" t="s">
         <v>85</v>
       </c>
@@ -1978,7 +2005,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7">
       <c r="A6" s="1" t="s">
         <v>87</v>
       </c>
@@ -2011,14 +2038,14 @@
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="3" width="15.625" customWidth="1"/>
-    <col min="4" max="6" width="7.625" customWidth="1"/>
-    <col min="7" max="7" width="15.625" customWidth="1"/>
+    <col min="1" max="3" width="15.6640625" customWidth="1"/>
+    <col min="4" max="6" width="7.6640625" customWidth="1"/>
+    <col min="7" max="7" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>89</v>
       </c>
@@ -2041,7 +2068,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7">
       <c r="A2" s="1" t="s">
         <v>90</v>
       </c>
@@ -2064,7 +2091,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7">
       <c r="A3" s="1" t="s">
         <v>91</v>
       </c>
@@ -2085,7 +2112,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7">
       <c r="A4" s="1" t="s">
         <v>92</v>
       </c>
@@ -2106,7 +2133,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7">
       <c r="A5" s="1" t="s">
         <v>93</v>
       </c>
@@ -2135,17 +2162,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F93CE324-7567-46F4-B0E6-A570E19390AA}">
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="2" max="2" width="9" customWidth="1"/>
-    <col min="3" max="3" width="18.25" customWidth="1"/>
+    <col min="3" max="3" width="18.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>112</v>
       </c>
@@ -2159,7 +2186,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
         <v>113</v>
       </c>
@@ -2171,7 +2198,7 @@
       </c>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
         <v>114</v>
       </c>
@@ -2185,7 +2212,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
         <v>115</v>
       </c>
@@ -2199,7 +2226,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4">
       <c r="A5" s="1" t="s">
         <v>116</v>
       </c>
@@ -2213,7 +2240,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4">
       <c r="A6" s="1" t="s">
         <v>117</v>
       </c>
@@ -2227,7 +2254,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
         <v>118</v>
       </c>
@@ -2241,7 +2268,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
         <v>119</v>
       </c>
@@ -2255,7 +2282,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
         <v>120</v>
       </c>
@@ -2269,7 +2296,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
         <v>141</v>
       </c>
@@ -2283,7 +2310,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4">
       <c r="A11" s="1" t="s">
         <v>142</v>
       </c>
@@ -2297,7 +2324,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4">
       <c r="A12" s="1" t="s">
         <v>143</v>
       </c>
@@ -2311,7 +2338,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4">
       <c r="A13" s="1" t="s">
         <v>144</v>
       </c>
@@ -2325,7 +2352,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4">
       <c r="A14" s="1" t="s">
         <v>145</v>
       </c>
@@ -2339,7 +2366,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4">
       <c r="A15" s="1" t="s">
         <v>146</v>
       </c>
@@ -2353,7 +2380,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4">
       <c r="A16" s="1" t="s">
         <v>147</v>
       </c>
@@ -2367,7 +2394,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4">
       <c r="A17" s="1" t="s">
         <v>148</v>
       </c>
@@ -2381,13 +2408,13 @@
         <v>162</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4">
       <c r="A19" s="1" t="s">
         <v>122</v>
       </c>
@@ -2397,13 +2424,13 @@
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>

</xml_diff>

<commit_message>
mul and div interface
</commit_message>
<xml_diff>
--- a/doc/24B-ISA.xlsx
+++ b/doc/24B-ISA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cathe\Documents\vlsi-cpu\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC8B378B-5EE5-4601-8955-1EDF49DCE559}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D316154F-514C-4B78-86BA-FE09D1406B54}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12168" xr2:uid="{300FB89C-001C-4516-AA49-DF67C212701F}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12168" activeTab="2" xr2:uid="{300FB89C-001C-4516-AA49-DF67C212701F}"/>
   </bookViews>
   <sheets>
     <sheet name="Inst" sheetId="1" r:id="rId1"/>
@@ -839,7 +839,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -849,6 +849,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -882,7 +888,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -893,6 +899,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1211,8 +1220,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBF12222-62EB-419B-868A-3559C151B634}">
   <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:E3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A16" sqref="A16:E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -1301,87 +1310,87 @@
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="4" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="4" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="4" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="4" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E9" s="4" t="s">
         <v>185</v>
       </c>
     </row>
@@ -1488,104 +1497,104 @@
       </c>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D16" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="E16" s="3" t="s">
+      <c r="E16" s="4" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="17" spans="1:5">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="D17" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="E17" s="3" t="s">
+      <c r="E17" s="4" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="18" spans="1:5">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="D18" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="E18" s="3" t="s">
+      <c r="E18" s="4" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19" s="3" t="s">
+      <c r="A19" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="D19" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="E19" s="3" t="s">
+      <c r="E19" s="4" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="20" spans="1:5">
-      <c r="A20" s="3" t="s">
+      <c r="A20" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C20" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="D20" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="E20" s="3" t="s">
+      <c r="E20" s="4" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="21" spans="1:5">
-      <c r="A21" s="3" t="s">
+      <c r="A21" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C21" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="D21" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="E21" s="3" t="s">
+      <c r="E21" s="4" t="s">
         <v>173</v>
       </c>
     </row>
@@ -2034,8 +2043,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B8EF21D-5FBA-4207-95A4-CD060BDF8CDE}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>

</xml_diff>